<commit_message>
Fixed BoM and CPL files during ordering.
</commit_message>
<xml_diff>
--- a/cam/W25Q-BRD-20221204-BoM.xlsx
+++ b/cam/W25Q-BRD-20221204-BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\KiCad\6.0\projects\W25Q-BRD\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF31AC9-6A12-4864-BA10-065122CBF87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E491A56-4D45-4E51-B36D-904EFAD8FBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="5508" windowWidth="16188" windowHeight="18684" xr2:uid="{62C69623-4926-4FBA-AC3A-AB79DE4B88D5}"/>
+    <workbookView xWindow="6612" yWindow="5676" windowWidth="16188" windowHeight="18684" xr2:uid="{62C69623-4926-4FBA-AC3A-AB79DE4B88D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
     <t>W25Q128JVSIQ</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>C25905</t>
+  </si>
+  <si>
+    <t>SOIC-8_208mil</t>
   </si>
 </sst>
 </file>
@@ -145,9 +145,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -155,13 +154,13 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -203,9 +202,9 @@
   <autoFilter ref="A1:D6" xr:uid="{BD12B529-E329-438D-A88B-6127A8E254E1}"/>
   <tableColumns count="4">
     <tableColumn id="2" xr3:uid="{441140BD-7209-48AC-BEA6-E6E4969290FB}" uniqueName="2" name="Designator" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6F28DFBF-6E79-4D85-870E-02508CCBCC35}" uniqueName="3" name="Footprint" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{562347DC-510C-4603-9FED-FF910BECA525}" uniqueName="5" name="Comment" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{3D90C788-A90C-4C54-A6C5-C15BB0A42941}" uniqueName="6" name="LCSC Part #" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{6F28DFBF-6E79-4D85-870E-02508CCBCC35}" uniqueName="3" name="Footprint" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{562347DC-510C-4603-9FED-FF910BECA525}" uniqueName="5" name="Comment" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{3D90C788-A90C-4C54-A6C5-C15BB0A42941}" uniqueName="6" name="LCSC Part #" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -511,7 +510,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,83 +525,83 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
+      <c r="D2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
+      <c r="D3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
+      <c r="D4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>